<commit_message>
fix in grade sheet
</commit_message>
<xml_diff>
--- a/Homework 4 grade sheet.xlsx
+++ b/Homework 4 grade sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Dropbox\BFOR 206\grading\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\code\bfor206-homework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA38BAC-87B2-49F2-998E-215D80F3FB2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D797873-4DA2-4AD5-8200-9E8A4EEAF646}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D73552CC-15B9-4A8F-ADCC-4ABA8EB54142}"/>
   </bookViews>
@@ -217,7 +217,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -428,24 +428,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="5" fillId="3" borderId="2" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="5" fillId="3" borderId="2" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -455,6 +443,18 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Accent1" xfId="5" builtinId="30"/>
@@ -522,7 +522,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -561,7 +561,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -600,7 +600,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -639,7 +639,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -678,7 +678,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -717,7 +717,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -756,7 +756,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -795,7 +795,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -834,7 +834,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -873,7 +873,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -912,7 +912,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -951,7 +951,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -984,10 +984,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1339,7 +1335,7 @@
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1354,36 +1350,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1425,7 +1421,7 @@
       <c r="M6" t="s">
         <v>17</v>
       </c>
-      <c r="N6" s="17" t="s">
+      <c r="N6" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1477,40 +1473,40 @@
       <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="4">
         <v>2</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="4">
         <v>2</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="4">
         <v>3</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="4">
         <v>1</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="4">
         <v>2</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="4">
         <v>2</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="4">
         <v>1</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="4">
         <v>1</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="4">
         <v>1</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="4">
         <v>1</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="4">
         <v>2</v>
       </c>
-      <c r="M8" s="6">
+      <c r="M8" s="4">
         <v>1</v>
       </c>
       <c r="N8">
@@ -1561,97 +1557,98 @@
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="8">
         <f>IF(B7="Yes", B8, 0)</f>
         <v>2</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="8">
         <f t="shared" ref="C11:M11" si="0">IF(C7="Yes", C8, 0)</f>
         <v>2</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K11" s="12">
+      <c r="K11" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M11" s="12">
+      <c r="M11" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N11" s="13">
+      <c r="N11" s="9">
         <f>N8</f>
         <v>-2</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="7">
+      <c r="B14" s="14"/>
+      <c r="C14" s="5">
         <f>SUM(Table1[[#Totals],[1.1]:[Documentation]])</f>
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="8">
+      <c r="B15" s="14"/>
+      <c r="C15" s="6">
         <f>C14/15</f>
         <v>0.13333333333333333</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S17" s="14"/>
+      <c r="S17" s="10"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="17"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="wzSPssWD2UPvMzA1pHs2p9tiqM53RjQVlE9oAQHWy2t+QhpsQSd8yz0dRVsRsL5MGHWbzWDsOvmDh7Esk+VOaw==" saltValue="g1QDEkLPkaF7w39hJplIBQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="9mXM/6GUpnCIlvAzsLP2m2ZTiiK5JBGNToai1DOCNtwJypaTw+u25GDWq3KWtZJVhuXlfWSB4HpVhsmHAuryiw==" saltValue="9xddWRsCknwh3crzQDmItw==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0"/>
   <protectedRanges>
-    <protectedRange sqref="B9:M10" name="filenames and notes"/>
+    <protectedRange sqref="N7" name="documentation"/>
+    <protectedRange sqref="B3:E4" name="Names"/>
     <protectedRange sqref="B7:M7" name="Completed"/>
-    <protectedRange sqref="B3:E4" name="Names"/>
+    <protectedRange sqref="B9:N10" name="filenames and notes"/>
   </protectedRanges>
   <mergeCells count="6">
     <mergeCell ref="A15:B15"/>
@@ -1710,44 +1707,44 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="3">
         <v>0</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="3">
         <v>-1</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>-2</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>-3</v>
       </c>
     </row>

</xml_diff>